<commit_message>
renew the excel file
</commit_message>
<xml_diff>
--- a/ExcelTables/GetLad.xlsx
+++ b/ExcelTables/GetLad.xlsx
@@ -1679,6 +1679,9 @@
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
+      <c r="B2" s="1">
+        <v>21.0</v>
+      </c>
       <c r="C2" s="1">
         <v>23.0</v>
       </c>
@@ -1687,6 +1690,9 @@
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
+      <c r="B3" s="1">
+        <v>5.0</v>
+      </c>
       <c r="C3" s="1">
         <v>11.0</v>
       </c>
@@ -1695,6 +1701,9 @@
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
+      <c r="B4" s="1">
+        <v>7.0</v>
+      </c>
       <c r="C4" s="1">
         <v>12.0</v>
       </c>
@@ -1703,6 +1712,9 @@
       <c r="A5" s="1">
         <v>4.0</v>
       </c>
+      <c r="B5" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C5" s="1">
         <v>26.0</v>
       </c>
@@ -1711,6 +1723,9 @@
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
+      <c r="B6" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C6" s="1">
         <v>10.0</v>
       </c>
@@ -1719,6 +1734,9 @@
       <c r="A7" s="1">
         <v>6.0</v>
       </c>
+      <c r="B7" s="1">
+        <v>4.0</v>
+      </c>
       <c r="C7" s="1">
         <v>18.0</v>
       </c>
@@ -1727,6 +1745,9 @@
       <c r="A8" s="1">
         <v>7.0</v>
       </c>
+      <c r="B8" s="1">
+        <v>26.0</v>
+      </c>
       <c r="C8" s="1">
         <v>24.0</v>
       </c>
@@ -1735,6 +1756,9 @@
       <c r="A9" s="1">
         <v>8.0</v>
       </c>
+      <c r="B9" s="1">
+        <v>16.0</v>
+      </c>
       <c r="C9" s="1">
         <v>3.0</v>
       </c>
@@ -1743,6 +1767,9 @@
       <c r="A10" s="1">
         <v>9.0</v>
       </c>
+      <c r="B10" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C10" s="1">
         <v>19.0</v>
       </c>
@@ -1751,6 +1778,9 @@
       <c r="A11" s="1">
         <v>10.0</v>
       </c>
+      <c r="B11" s="1">
+        <v>27.0</v>
+      </c>
       <c r="C11" s="1">
         <v>30.0</v>
       </c>
@@ -1759,6 +1789,9 @@
       <c r="A12" s="1">
         <v>11.0</v>
       </c>
+      <c r="B12" s="1">
+        <v>21.0</v>
+      </c>
       <c r="C12" s="1">
         <v>28.0</v>
       </c>
@@ -1767,6 +1800,9 @@
       <c r="A13" s="1">
         <v>12.0</v>
       </c>
+      <c r="B13" s="1">
+        <v>20.0</v>
+      </c>
       <c r="C13" s="1">
         <v>1.0</v>
       </c>
@@ -1775,6 +1811,9 @@
       <c r="A14" s="1">
         <v>13.0</v>
       </c>
+      <c r="B14" s="1">
+        <v>9.0</v>
+      </c>
       <c r="C14" s="1">
         <v>12.0</v>
       </c>
@@ -1783,6 +1822,9 @@
       <c r="A15" s="1">
         <v>14.0</v>
       </c>
+      <c r="B15" s="1">
+        <v>26.0</v>
+      </c>
       <c r="C15" s="1">
         <v>8.0</v>
       </c>
@@ -1791,6 +1833,9 @@
       <c r="A16" s="1">
         <v>15.0</v>
       </c>
+      <c r="B16" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C16" s="1">
         <v>14.0</v>
       </c>
@@ -1799,6 +1844,9 @@
       <c r="A17" s="1">
         <v>16.0</v>
       </c>
+      <c r="B17" s="1">
+        <v>29.0</v>
+      </c>
       <c r="C17" s="1">
         <v>18.0</v>
       </c>
@@ -1807,6 +1855,9 @@
       <c r="A18" s="1">
         <v>17.0</v>
       </c>
+      <c r="B18" s="1">
+        <v>16.0</v>
+      </c>
       <c r="C18" s="1">
         <v>20.0</v>
       </c>
@@ -1815,6 +1866,9 @@
       <c r="A19" s="1">
         <v>18.0</v>
       </c>
+      <c r="B19" s="1">
+        <v>26.0</v>
+      </c>
       <c r="C19" s="1">
         <v>21.0</v>
       </c>
@@ -1823,6 +1877,9 @@
       <c r="A20" s="1">
         <v>19.0</v>
       </c>
+      <c r="B20" s="1">
+        <v>2.0</v>
+      </c>
       <c r="C20" s="1">
         <v>21.0</v>
       </c>
@@ -1831,6 +1888,9 @@
       <c r="A21" s="1">
         <v>20.0</v>
       </c>
+      <c r="B21" s="1">
+        <v>30.0</v>
+      </c>
       <c r="C21" s="1">
         <v>28.0</v>
       </c>
@@ -1839,6 +1899,9 @@
       <c r="A22" s="1">
         <v>21.0</v>
       </c>
+      <c r="B22" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C22" s="1">
         <v>2.0</v>
       </c>
@@ -1847,6 +1910,9 @@
       <c r="A23" s="1">
         <v>22.0</v>
       </c>
+      <c r="B23" s="1">
+        <v>19.0</v>
+      </c>
       <c r="C23" s="1">
         <v>7.0</v>
       </c>
@@ -1855,6 +1921,9 @@
       <c r="A24" s="1">
         <v>23.0</v>
       </c>
+      <c r="B24" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C24" s="1">
         <v>13.0</v>
       </c>
@@ -1863,6 +1932,9 @@
       <c r="A25" s="1">
         <v>24.0</v>
       </c>
+      <c r="B25" s="2">
+        <v>27.0</v>
+      </c>
       <c r="C25" s="1">
         <v>30.0</v>
       </c>
@@ -1871,6 +1943,9 @@
       <c r="A26" s="1">
         <v>25.0</v>
       </c>
+      <c r="B26" s="1">
+        <v>6.0</v>
+      </c>
       <c r="C26" s="1">
         <v>15.0</v>
       </c>
@@ -1879,6 +1954,9 @@
       <c r="A27" s="1">
         <v>26.0</v>
       </c>
+      <c r="B27" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C27" s="1">
         <v>13.0</v>
       </c>
@@ -1887,6 +1965,9 @@
       <c r="A28" s="1">
         <v>27.0</v>
       </c>
+      <c r="B28" s="2">
+        <v>28.0</v>
+      </c>
       <c r="C28" s="1">
         <v>28.0</v>
       </c>
@@ -1895,6 +1976,9 @@
       <c r="A29" s="1">
         <v>28.0</v>
       </c>
+      <c r="B29" s="1">
+        <v>22.0</v>
+      </c>
       <c r="C29" s="1">
         <v>14.0</v>
       </c>
@@ -1903,6 +1987,9 @@
       <c r="A30" s="1">
         <v>29.0</v>
       </c>
+      <c r="B30" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C30" s="1">
         <v>9.0</v>
       </c>
@@ -1911,6 +1998,9 @@
       <c r="A31" s="1">
         <v>30.0</v>
       </c>
+      <c r="B31" s="1">
+        <v>24.0</v>
+      </c>
       <c r="C31" s="1">
         <v>16.0</v>
       </c>
@@ -1919,6 +2009,9 @@
       <c r="A32" s="1">
         <v>31.0</v>
       </c>
+      <c r="B32" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C32" s="1">
         <v>13.0</v>
       </c>
@@ -1927,6 +2020,9 @@
       <c r="A33" s="1">
         <v>32.0</v>
       </c>
+      <c r="B33" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C33" s="1">
         <v>8.0</v>
       </c>
@@ -1935,6 +2031,9 @@
       <c r="A34" s="1">
         <v>33.0</v>
       </c>
+      <c r="B34" s="1">
+        <v>24.0</v>
+      </c>
       <c r="C34" s="1">
         <v>15.0</v>
       </c>
@@ -1943,6 +2042,9 @@
       <c r="A35" s="1">
         <v>34.0</v>
       </c>
+      <c r="B35" s="1">
+        <v>1.0</v>
+      </c>
       <c r="C35" s="1">
         <v>10.0</v>
       </c>
@@ -1951,6 +2053,9 @@
       <c r="A36" s="1">
         <v>35.0</v>
       </c>
+      <c r="B36" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C36" s="1">
         <v>25.0</v>
       </c>
@@ -1959,6 +2064,9 @@
       <c r="A37" s="1">
         <v>36.0</v>
       </c>
+      <c r="B37" s="1">
+        <v>30.0</v>
+      </c>
       <c r="C37" s="1">
         <v>29.0</v>
       </c>
@@ -1967,6 +2075,9 @@
       <c r="A38" s="1">
         <v>37.0</v>
       </c>
+      <c r="B38" s="1">
+        <v>28.0</v>
+      </c>
       <c r="C38" s="1">
         <v>17.0</v>
       </c>
@@ -1975,6 +2086,9 @@
       <c r="A39" s="1">
         <v>38.0</v>
       </c>
+      <c r="B39" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C39" s="1">
         <v>5.0</v>
       </c>
@@ -1983,6 +2097,9 @@
       <c r="A40" s="1">
         <v>39.0</v>
       </c>
+      <c r="B40" s="1">
+        <v>7.0</v>
+      </c>
       <c r="C40" s="1">
         <v>27.0</v>
       </c>
@@ -1991,6 +2108,9 @@
       <c r="A41" s="1">
         <v>40.0</v>
       </c>
+      <c r="B41" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C41" s="1">
         <v>7.0</v>
       </c>
@@ -1999,6 +2119,9 @@
       <c r="A42" s="1">
         <v>41.0</v>
       </c>
+      <c r="B42" s="2">
+        <v>30.0</v>
+      </c>
       <c r="C42" s="1">
         <v>19.0</v>
       </c>
@@ -2007,6 +2130,9 @@
       <c r="A43" s="1">
         <v>42.0</v>
       </c>
+      <c r="B43" s="1">
+        <v>26.0</v>
+      </c>
       <c r="C43" s="1">
         <v>7.0</v>
       </c>
@@ -2015,6 +2141,9 @@
       <c r="A44" s="1">
         <v>43.0</v>
       </c>
+      <c r="B44" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C44" s="1">
         <v>4.0</v>
       </c>
@@ -2023,6 +2152,9 @@
       <c r="A45" s="1">
         <v>44.0</v>
       </c>
+      <c r="B45" s="2">
+        <v>29.0</v>
+      </c>
       <c r="C45" s="1">
         <v>23.0</v>
       </c>
@@ -2031,6 +2163,9 @@
       <c r="A46" s="1">
         <v>45.0</v>
       </c>
+      <c r="B46" s="1">
+        <v>4.0</v>
+      </c>
       <c r="C46" s="1">
         <v>25.0</v>
       </c>
@@ -2039,6 +2174,9 @@
       <c r="A47" s="1">
         <v>46.0</v>
       </c>
+      <c r="B47" s="1">
+        <v>24.0</v>
+      </c>
       <c r="C47" s="1">
         <v>22.0</v>
       </c>
@@ -2047,6 +2185,9 @@
       <c r="A48" s="1">
         <v>47.0</v>
       </c>
+      <c r="B48" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C48" s="1">
         <v>22.0</v>
       </c>
@@ -2055,6 +2196,9 @@
       <c r="A49" s="1">
         <v>48.0</v>
       </c>
+      <c r="B49" s="1">
+        <v>27.0</v>
+      </c>
       <c r="C49" s="1">
         <v>23.0</v>
       </c>
@@ -2063,6 +2207,9 @@
       <c r="A50" s="1">
         <v>49.0</v>
       </c>
+      <c r="B50" s="1">
+        <v>17.0</v>
+      </c>
       <c r="C50" s="1">
         <v>27.0</v>
       </c>
@@ -2071,6 +2218,9 @@
       <c r="A51" s="1">
         <v>50.0</v>
       </c>
+      <c r="B51" s="1">
+        <v>8.0</v>
+      </c>
       <c r="C51" s="1">
         <v>11.0</v>
       </c>
@@ -2079,6 +2229,9 @@
       <c r="A52" s="1">
         <v>51.0</v>
       </c>
+      <c r="B52" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C52" s="1">
         <v>21.0</v>
       </c>
@@ -2087,6 +2240,9 @@
       <c r="A53" s="1">
         <v>52.0</v>
       </c>
+      <c r="B53" s="1">
+        <v>16.0</v>
+      </c>
       <c r="C53" s="1">
         <v>10.0</v>
       </c>
@@ -2095,6 +2251,9 @@
       <c r="A54" s="1">
         <v>53.0</v>
       </c>
+      <c r="B54" s="1">
+        <v>1.0</v>
+      </c>
       <c r="C54" s="1">
         <v>15.0</v>
       </c>
@@ -2103,6 +2262,9 @@
       <c r="A55" s="1">
         <v>54.0</v>
       </c>
+      <c r="B55" s="1">
+        <v>3.0</v>
+      </c>
       <c r="C55" s="1">
         <v>9.0</v>
       </c>
@@ -2111,6 +2273,9 @@
       <c r="A56" s="1">
         <v>55.0</v>
       </c>
+      <c r="B56" s="1">
+        <v>25.0</v>
+      </c>
       <c r="C56" s="1">
         <v>8.0</v>
       </c>
@@ -2119,6 +2284,9 @@
       <c r="A57" s="1">
         <v>56.0</v>
       </c>
+      <c r="B57" s="1">
+        <v>8.0</v>
+      </c>
       <c r="C57" s="1">
         <v>25.0</v>
       </c>
@@ -2127,6 +2295,9 @@
       <c r="A58" s="1">
         <v>57.0</v>
       </c>
+      <c r="B58" s="1">
+        <v>25.0</v>
+      </c>
       <c r="C58" s="1">
         <v>27.0</v>
       </c>
@@ -2135,6 +2306,9 @@
       <c r="A59" s="1">
         <v>58.0</v>
       </c>
+      <c r="B59" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C59" s="1">
         <v>3.0</v>
       </c>
@@ -2143,6 +2317,9 @@
       <c r="A60" s="1">
         <v>59.0</v>
       </c>
+      <c r="B60" s="1">
+        <v>30.0</v>
+      </c>
       <c r="C60" s="1">
         <v>14.0</v>
       </c>
@@ -2151,6 +2328,9 @@
       <c r="A61" s="1">
         <v>60.0</v>
       </c>
+      <c r="B61" s="1">
+        <v>19.0</v>
+      </c>
       <c r="C61" s="1">
         <v>3.0</v>
       </c>
@@ -2159,6 +2339,9 @@
       <c r="A62" s="1">
         <v>61.0</v>
       </c>
+      <c r="B62" s="2">
+        <v>25.0</v>
+      </c>
       <c r="C62" s="1">
         <v>12.0</v>
       </c>
@@ -2167,6 +2350,9 @@
       <c r="A63" s="1">
         <v>62.0</v>
       </c>
+      <c r="B63" s="1">
+        <v>17.0</v>
+      </c>
       <c r="C63" s="1">
         <v>1.0</v>
       </c>
@@ -2175,6 +2361,9 @@
       <c r="A64" s="1">
         <v>63.0</v>
       </c>
+      <c r="B64" s="1">
+        <v>22.0</v>
+      </c>
       <c r="C64" s="1">
         <v>5.0</v>
       </c>
@@ -2183,6 +2372,9 @@
       <c r="A65" s="1">
         <v>64.0</v>
       </c>
+      <c r="B65" s="1">
+        <v>19.0</v>
+      </c>
       <c r="C65" s="1">
         <v>17.0</v>
       </c>
@@ -2191,6 +2383,9 @@
       <c r="A66" s="1">
         <v>65.0</v>
       </c>
+      <c r="B66" s="1">
+        <v>17.0</v>
+      </c>
       <c r="C66" s="1">
         <v>2.0</v>
       </c>
@@ -2199,6 +2394,9 @@
       <c r="A67" s="1">
         <v>66.0</v>
       </c>
+      <c r="B67" s="1">
+        <v>29.0</v>
+      </c>
       <c r="C67" s="1">
         <v>5.0</v>
       </c>
@@ -2207,6 +2405,9 @@
       <c r="A68" s="1">
         <v>67.0</v>
       </c>
+      <c r="B68" s="1">
+        <v>7.0</v>
+      </c>
       <c r="C68" s="1">
         <v>29.0</v>
       </c>
@@ -2215,6 +2416,9 @@
       <c r="A69" s="1">
         <v>68.0</v>
       </c>
+      <c r="B69" s="1">
+        <v>5.0</v>
+      </c>
       <c r="C69" s="1">
         <v>7.0</v>
       </c>
@@ -2223,6 +2427,9 @@
       <c r="A70" s="1">
         <v>69.0</v>
       </c>
+      <c r="B70" s="1">
+        <v>23.0</v>
+      </c>
       <c r="C70" s="1">
         <v>6.0</v>
       </c>
@@ -2231,6 +2438,9 @@
       <c r="A71" s="1">
         <v>70.0</v>
       </c>
+      <c r="B71" s="1">
+        <v>6.0</v>
+      </c>
       <c r="C71" s="1">
         <v>6.0</v>
       </c>
@@ -2239,6 +2449,9 @@
       <c r="A72" s="1">
         <v>71.0</v>
       </c>
+      <c r="B72" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C72" s="1">
         <v>2.0</v>
       </c>
@@ -2247,6 +2460,9 @@
       <c r="A73" s="1">
         <v>72.0</v>
       </c>
+      <c r="B73" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C73" s="1">
         <v>27.0</v>
       </c>
@@ -2255,6 +2471,9 @@
       <c r="A74" s="1">
         <v>73.0</v>
       </c>
+      <c r="B74" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C74" s="1">
         <v>17.0</v>
       </c>
@@ -2263,6 +2482,9 @@
       <c r="A75" s="1">
         <v>74.0</v>
       </c>
+      <c r="B75" s="1">
+        <v>8.0</v>
+      </c>
       <c r="C75" s="1">
         <v>30.0</v>
       </c>
@@ -2271,6 +2493,9 @@
       <c r="A76" s="1">
         <v>75.0</v>
       </c>
+      <c r="B76" s="1">
+        <v>9.0</v>
+      </c>
       <c r="C76" s="1">
         <v>16.0</v>
       </c>
@@ -2279,6 +2504,9 @@
       <c r="A77" s="1">
         <v>76.0</v>
       </c>
+      <c r="B77" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C77" s="1">
         <v>29.0</v>
       </c>
@@ -2287,6 +2515,9 @@
       <c r="A78" s="1">
         <v>77.0</v>
       </c>
+      <c r="B78" s="1">
+        <v>9.0</v>
+      </c>
       <c r="C78" s="1">
         <v>6.0</v>
       </c>
@@ -2295,6 +2526,9 @@
       <c r="A79" s="1">
         <v>78.0</v>
       </c>
+      <c r="B79" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C79" s="1">
         <v>1.0</v>
       </c>
@@ -2303,6 +2537,9 @@
       <c r="A80" s="1">
         <v>79.0</v>
       </c>
+      <c r="B80" s="1">
+        <v>16.0</v>
+      </c>
       <c r="C80" s="1">
         <v>26.0</v>
       </c>
@@ -2311,6 +2548,9 @@
       <c r="A81" s="1">
         <v>80.0</v>
       </c>
+      <c r="B81" s="1">
+        <v>17.0</v>
+      </c>
       <c r="C81" s="1">
         <v>9.0</v>
       </c>
@@ -2319,6 +2559,9 @@
       <c r="A82" s="1">
         <v>81.0</v>
       </c>
+      <c r="B82" s="1">
+        <v>22.0</v>
+      </c>
       <c r="C82" s="1">
         <v>26.0</v>
       </c>
@@ -2327,6 +2570,9 @@
       <c r="A83" s="1">
         <v>82.0</v>
       </c>
+      <c r="B83" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C83" s="1">
         <v>8.0</v>
       </c>
@@ -2335,6 +2581,9 @@
       <c r="A84" s="1">
         <v>83.0</v>
       </c>
+      <c r="B84" s="1">
+        <v>28.0</v>
+      </c>
       <c r="C84" s="1">
         <v>24.0</v>
       </c>
@@ -2343,6 +2592,9 @@
       <c r="A85" s="1">
         <v>84.0</v>
       </c>
+      <c r="B85" s="1">
+        <v>23.0</v>
+      </c>
       <c r="C85" s="1">
         <v>20.0</v>
       </c>
@@ -2351,6 +2603,9 @@
       <c r="A86" s="1">
         <v>85.0</v>
       </c>
+      <c r="B86" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C86" s="1">
         <v>19.0</v>
       </c>
@@ -2359,6 +2614,9 @@
       <c r="A87" s="1">
         <v>86.0</v>
       </c>
+      <c r="B87" s="1">
+        <v>20.0</v>
+      </c>
       <c r="C87" s="1">
         <v>24.0</v>
       </c>
@@ -2367,6 +2625,9 @@
       <c r="A88" s="1">
         <v>87.0</v>
       </c>
+      <c r="B88" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C88" s="1">
         <v>28.0</v>
       </c>
@@ -2375,6 +2636,9 @@
       <c r="A89" s="1">
         <v>88.0</v>
       </c>
+      <c r="B89" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C89" s="1">
         <v>20.0</v>
       </c>
@@ -2383,6 +2647,9 @@
       <c r="A90" s="1">
         <v>89.0</v>
       </c>
+      <c r="B90" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C90" s="1">
         <v>11.0</v>
       </c>
@@ -2391,6 +2658,9 @@
       <c r="A91" s="1">
         <v>90.0</v>
       </c>
+      <c r="B91" s="1">
+        <v>3.0</v>
+      </c>
       <c r="C91" s="1">
         <v>9.0</v>
       </c>
@@ -2399,6 +2669,9 @@
       <c r="A92" s="1">
         <v>91.0</v>
       </c>
+      <c r="B92" s="1">
+        <v>25.0</v>
+      </c>
       <c r="C92" s="1">
         <v>18.0</v>
       </c>
@@ -2407,6 +2680,9 @@
       <c r="A93" s="1">
         <v>92.0</v>
       </c>
+      <c r="B93" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C93" s="1">
         <v>29.0</v>
       </c>
@@ -2415,6 +2691,9 @@
       <c r="A94" s="1">
         <v>93.0</v>
       </c>
+      <c r="B94" s="1">
+        <v>27.0</v>
+      </c>
       <c r="C94" s="1">
         <v>30.0</v>
       </c>
@@ -2423,6 +2702,9 @@
       <c r="A95" s="1">
         <v>94.0</v>
       </c>
+      <c r="B95" s="1">
+        <v>29.0</v>
+      </c>
       <c r="C95" s="1">
         <v>4.0</v>
       </c>
@@ -2431,6 +2713,9 @@
       <c r="A96" s="1">
         <v>95.0</v>
       </c>
+      <c r="B96" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C96" s="1">
         <v>22.0</v>
       </c>
@@ -2439,6 +2724,9 @@
       <c r="A97" s="1">
         <v>96.0</v>
       </c>
+      <c r="B97" s="1">
+        <v>28.0</v>
+      </c>
       <c r="C97" s="1">
         <v>16.0</v>
       </c>
@@ -2447,6 +2735,9 @@
       <c r="A98" s="1">
         <v>97.0</v>
       </c>
+      <c r="B98" s="1">
+        <v>23.0</v>
+      </c>
       <c r="C98" s="1">
         <v>26.0</v>
       </c>
@@ -2455,6 +2746,9 @@
       <c r="A99" s="1">
         <v>98.0</v>
       </c>
+      <c r="B99" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C99" s="1">
         <v>4.0</v>
       </c>
@@ -2463,6 +2757,9 @@
       <c r="A100" s="1">
         <v>99.0</v>
       </c>
+      <c r="B100" s="2">
+        <v>26.0</v>
+      </c>
       <c r="C100" s="1">
         <v>25.0</v>
       </c>
@@ -2470,6 +2767,9 @@
     <row r="101">
       <c r="A101" s="1">
         <v>100.0</v>
+      </c>
+      <c r="B101" s="1">
+        <v>2.0</v>
       </c>
       <c r="C101" s="1">
         <v>24.0</v>
@@ -2505,6 +2805,9 @@
       <c r="A2" s="1">
         <v>1.0</v>
       </c>
+      <c r="B2" s="1">
+        <v>8.0</v>
+      </c>
       <c r="C2" s="1">
         <v>15.0</v>
       </c>
@@ -2513,6 +2816,9 @@
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
+      <c r="B3" s="1">
+        <v>1.0</v>
+      </c>
       <c r="C3" s="1">
         <v>20.0</v>
       </c>
@@ -2521,6 +2827,9 @@
       <c r="A4" s="1">
         <v>3.0</v>
       </c>
+      <c r="B4" s="1">
+        <v>17.0</v>
+      </c>
       <c r="C4" s="1">
         <v>9.0</v>
       </c>
@@ -2529,6 +2838,9 @@
       <c r="A5" s="1">
         <v>4.0</v>
       </c>
+      <c r="B5" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C5" s="1">
         <v>10.0</v>
       </c>
@@ -2537,6 +2849,9 @@
       <c r="A6" s="1">
         <v>5.0</v>
       </c>
+      <c r="B6" s="1">
+        <v>20.0</v>
+      </c>
       <c r="C6" s="1">
         <v>30.0</v>
       </c>
@@ -2545,6 +2860,9 @@
       <c r="A7" s="1">
         <v>6.0</v>
       </c>
+      <c r="B7" s="1">
+        <v>5.0</v>
+      </c>
       <c r="C7" s="1">
         <v>20.0</v>
       </c>
@@ -2553,6 +2871,9 @@
       <c r="A8" s="1">
         <v>7.0</v>
       </c>
+      <c r="B8" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C8" s="1">
         <v>22.0</v>
       </c>
@@ -2561,6 +2882,9 @@
       <c r="A9" s="1">
         <v>8.0</v>
       </c>
+      <c r="B9" s="1">
+        <v>5.0</v>
+      </c>
       <c r="C9" s="1">
         <v>27.0</v>
       </c>
@@ -2569,6 +2893,9 @@
       <c r="A10" s="1">
         <v>9.0</v>
       </c>
+      <c r="B10" s="1">
+        <v>27.0</v>
+      </c>
       <c r="C10" s="1">
         <v>1.0</v>
       </c>
@@ -2577,6 +2904,9 @@
       <c r="A11" s="1">
         <v>10.0</v>
       </c>
+      <c r="B11" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C11" s="1">
         <v>1.0</v>
       </c>
@@ -2585,6 +2915,9 @@
       <c r="A12" s="1">
         <v>11.0</v>
       </c>
+      <c r="B12" s="1">
+        <v>19.0</v>
+      </c>
       <c r="C12" s="1">
         <v>3.0</v>
       </c>
@@ -2593,6 +2926,9 @@
       <c r="A13" s="1">
         <v>12.0</v>
       </c>
+      <c r="B13" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C13" s="1">
         <v>14.0</v>
       </c>
@@ -2601,6 +2937,9 @@
       <c r="A14" s="1">
         <v>13.0</v>
       </c>
+      <c r="B14" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C14" s="1">
         <v>4.0</v>
       </c>
@@ -2609,6 +2948,9 @@
       <c r="A15" s="1">
         <v>14.0</v>
       </c>
+      <c r="B15" s="1">
+        <v>16.0</v>
+      </c>
       <c r="C15" s="1">
         <v>7.0</v>
       </c>
@@ -2617,6 +2959,9 @@
       <c r="A16" s="1">
         <v>15.0</v>
       </c>
+      <c r="B16" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C16" s="1">
         <v>21.0</v>
       </c>
@@ -2625,6 +2970,9 @@
       <c r="A17" s="1">
         <v>16.0</v>
       </c>
+      <c r="B17" s="1">
+        <v>20.0</v>
+      </c>
       <c r="C17" s="1">
         <v>29.0</v>
       </c>
@@ -2633,6 +2981,9 @@
       <c r="A18" s="1">
         <v>17.0</v>
       </c>
+      <c r="B18" s="1">
+        <v>7.0</v>
+      </c>
       <c r="C18" s="1">
         <v>26.0</v>
       </c>
@@ -2641,6 +2992,9 @@
       <c r="A19" s="1">
         <v>18.0</v>
       </c>
+      <c r="B19" s="1">
+        <v>19.0</v>
+      </c>
       <c r="C19" s="1">
         <v>30.0</v>
       </c>
@@ -2649,6 +3003,9 @@
       <c r="A20" s="1">
         <v>19.0</v>
       </c>
+      <c r="B20" s="1">
+        <v>3.0</v>
+      </c>
       <c r="C20" s="1">
         <v>19.0</v>
       </c>
@@ -2657,6 +3014,9 @@
       <c r="A21" s="1">
         <v>20.0</v>
       </c>
+      <c r="B21" s="1">
+        <v>21.0</v>
+      </c>
       <c r="C21" s="1">
         <v>14.0</v>
       </c>
@@ -2665,6 +3025,9 @@
       <c r="A22" s="1">
         <v>21.0</v>
       </c>
+      <c r="B22" s="1">
+        <v>1.0</v>
+      </c>
       <c r="C22" s="1">
         <v>28.0</v>
       </c>
@@ -2673,6 +3036,9 @@
       <c r="A23" s="1">
         <v>22.0</v>
       </c>
+      <c r="B23" s="1">
+        <v>4.0</v>
+      </c>
       <c r="C23" s="1">
         <v>11.0</v>
       </c>
@@ -2681,6 +3047,9 @@
       <c r="A24" s="1">
         <v>23.0</v>
       </c>
+      <c r="B24" s="1">
+        <v>17.0</v>
+      </c>
       <c r="C24" s="1">
         <v>29.0</v>
       </c>
@@ -2689,6 +3058,9 @@
       <c r="A25" s="1">
         <v>24.0</v>
       </c>
+      <c r="B25" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C25" s="1">
         <v>13.0</v>
       </c>
@@ -2697,6 +3069,9 @@
       <c r="A26" s="1">
         <v>25.0</v>
       </c>
+      <c r="B26" s="1">
+        <v>2.0</v>
+      </c>
       <c r="C26" s="1">
         <v>2.0</v>
       </c>
@@ -2705,6 +3080,9 @@
       <c r="A27" s="1">
         <v>26.0</v>
       </c>
+      <c r="B27" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C27" s="1">
         <v>21.0</v>
       </c>
@@ -2713,6 +3091,9 @@
       <c r="A28" s="1">
         <v>27.0</v>
       </c>
+      <c r="B28" s="1">
+        <v>15.0</v>
+      </c>
       <c r="C28" s="1">
         <v>22.0</v>
       </c>
@@ -2721,6 +3102,9 @@
       <c r="A29" s="1">
         <v>28.0</v>
       </c>
+      <c r="B29" s="1">
+        <v>28.0</v>
+      </c>
       <c r="C29" s="1">
         <v>15.0</v>
       </c>
@@ -2729,6 +3113,9 @@
       <c r="A30" s="1">
         <v>29.0</v>
       </c>
+      <c r="B30" s="1">
+        <v>19.0</v>
+      </c>
       <c r="C30" s="1">
         <v>17.0</v>
       </c>
@@ -2737,6 +3124,9 @@
       <c r="A31" s="1">
         <v>30.0</v>
       </c>
+      <c r="B31" s="1">
+        <v>28.0</v>
+      </c>
       <c r="C31" s="1">
         <v>12.0</v>
       </c>
@@ -2745,6 +3135,9 @@
       <c r="A32" s="1">
         <v>31.0</v>
       </c>
+      <c r="B32" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C32" s="1">
         <v>16.0</v>
       </c>
@@ -2753,6 +3146,9 @@
       <c r="A33" s="1">
         <v>32.0</v>
       </c>
+      <c r="B33" s="1">
+        <v>11.0</v>
+      </c>
       <c r="C33" s="1">
         <v>5.0</v>
       </c>
@@ -2761,6 +3157,9 @@
       <c r="A34" s="1">
         <v>33.0</v>
       </c>
+      <c r="B34" s="1">
+        <v>12.0</v>
+      </c>
       <c r="C34" s="1">
         <v>24.0</v>
       </c>
@@ -2769,6 +3168,9 @@
       <c r="A35" s="1">
         <v>34.0</v>
       </c>
+      <c r="B35" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C35" s="1">
         <v>16.0</v>
       </c>
@@ -2777,6 +3179,9 @@
       <c r="A36" s="1">
         <v>35.0</v>
       </c>
+      <c r="B36" s="1">
+        <v>18.0</v>
+      </c>
       <c r="C36" s="1">
         <v>17.0</v>
       </c>
@@ -2785,6 +3190,9 @@
       <c r="A37" s="1">
         <v>36.0</v>
       </c>
+      <c r="B37" s="1">
+        <v>9.0</v>
+      </c>
       <c r="C37" s="1">
         <v>2.0</v>
       </c>
@@ -2793,6 +3201,9 @@
       <c r="A38" s="1">
         <v>37.0</v>
       </c>
+      <c r="B38" s="1">
+        <v>25.0</v>
+      </c>
       <c r="C38" s="1">
         <v>8.0</v>
       </c>
@@ -2801,6 +3212,9 @@
       <c r="A39" s="1">
         <v>38.0</v>
       </c>
+      <c r="B39" s="1">
+        <v>21.0</v>
+      </c>
       <c r="C39" s="1">
         <v>24.0</v>
       </c>
@@ -2809,6 +3223,9 @@
       <c r="A40" s="1">
         <v>39.0</v>
       </c>
+      <c r="B40" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C40" s="1">
         <v>23.0</v>
       </c>
@@ -2817,6 +3234,9 @@
       <c r="A41" s="1">
         <v>40.0</v>
       </c>
+      <c r="B41" s="1">
+        <v>3.0</v>
+      </c>
       <c r="C41" s="1">
         <v>25.0</v>
       </c>
@@ -2825,6 +3245,9 @@
       <c r="A42" s="1">
         <v>41.0</v>
       </c>
+      <c r="B42" s="1">
+        <v>22.0</v>
+      </c>
       <c r="C42" s="1">
         <v>27.0</v>
       </c>
@@ -2833,6 +3256,9 @@
       <c r="A43" s="1">
         <v>42.0</v>
       </c>
+      <c r="B43" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C43" s="1">
         <v>25.0</v>
       </c>
@@ -2841,6 +3267,9 @@
       <c r="A44" s="1">
         <v>43.0</v>
       </c>
+      <c r="B44" s="1">
+        <v>6.0</v>
+      </c>
       <c r="C44" s="1">
         <v>9.0</v>
       </c>
@@ -2849,6 +3278,9 @@
       <c r="A45" s="1">
         <v>44.0</v>
       </c>
+      <c r="B45" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C45" s="1">
         <v>18.0</v>
       </c>
@@ -2857,6 +3289,9 @@
       <c r="A46" s="1">
         <v>45.0</v>
       </c>
+      <c r="B46" s="1">
+        <v>21.0</v>
+      </c>
       <c r="C46" s="1">
         <v>5.0</v>
       </c>
@@ -2865,6 +3300,9 @@
       <c r="A47" s="1">
         <v>46.0</v>
       </c>
+      <c r="B47" s="1">
+        <v>6.0</v>
+      </c>
       <c r="C47" s="1">
         <v>11.0</v>
       </c>
@@ -2873,6 +3311,9 @@
       <c r="A48" s="1">
         <v>47.0</v>
       </c>
+      <c r="B48" s="1">
+        <v>8.0</v>
+      </c>
       <c r="C48" s="1">
         <v>8.0</v>
       </c>
@@ -2881,6 +3322,9 @@
       <c r="A49" s="1">
         <v>48.0</v>
       </c>
+      <c r="B49" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C49" s="1">
         <v>3.0</v>
       </c>
@@ -2889,6 +3333,9 @@
       <c r="A50" s="1">
         <v>49.0</v>
       </c>
+      <c r="B50" s="1">
+        <v>2.0</v>
+      </c>
       <c r="C50" s="1">
         <v>13.0</v>
       </c>
@@ -2897,6 +3344,9 @@
       <c r="A51" s="1">
         <v>50.0</v>
       </c>
+      <c r="B51" s="1">
+        <v>7.0</v>
+      </c>
       <c r="C51" s="1">
         <v>12.0</v>
       </c>
@@ -2905,6 +3355,9 @@
       <c r="A52" s="1">
         <v>51.0</v>
       </c>
+      <c r="B52" s="1">
+        <v>20.0</v>
+      </c>
       <c r="C52" s="1">
         <v>7.0</v>
       </c>
@@ -2913,6 +3366,9 @@
       <c r="A53" s="1">
         <v>52.0</v>
       </c>
+      <c r="B53" s="1">
+        <v>16.0</v>
+      </c>
       <c r="C53" s="1">
         <v>4.0</v>
       </c>
@@ -2921,6 +3377,9 @@
       <c r="A54" s="1">
         <v>53.0</v>
       </c>
+      <c r="B54" s="1">
+        <v>14.0</v>
+      </c>
       <c r="C54" s="1">
         <v>6.0</v>
       </c>
@@ -2929,6 +3388,9 @@
       <c r="A55" s="1">
         <v>54.0</v>
       </c>
+      <c r="B55" s="1">
+        <v>4.0</v>
+      </c>
       <c r="C55" s="1">
         <v>10.0</v>
       </c>
@@ -2937,6 +3399,9 @@
       <c r="A56" s="1">
         <v>55.0</v>
       </c>
+      <c r="B56" s="1">
+        <v>23.0</v>
+      </c>
       <c r="C56" s="1">
         <v>28.0</v>
       </c>
@@ -2945,6 +3410,9 @@
       <c r="A57" s="1">
         <v>56.0</v>
       </c>
+      <c r="B57" s="1">
+        <v>22.0</v>
+      </c>
       <c r="C57" s="1">
         <v>18.0</v>
       </c>
@@ -2953,6 +3421,9 @@
       <c r="A58" s="1">
         <v>57.0</v>
       </c>
+      <c r="B58" s="1">
+        <v>13.0</v>
+      </c>
       <c r="C58" s="1">
         <v>6.0</v>
       </c>
@@ -2961,6 +3432,9 @@
       <c r="A59" s="1">
         <v>58.0</v>
       </c>
+      <c r="B59" s="1">
+        <v>30.0</v>
+      </c>
       <c r="C59" s="1">
         <v>26.0</v>
       </c>
@@ -2969,6 +3443,9 @@
       <c r="A60" s="1">
         <v>59.0</v>
       </c>
+      <c r="B60" s="1">
+        <v>10.0</v>
+      </c>
       <c r="C60" s="1">
         <v>19.0</v>
       </c>
@@ -2976,6 +3453,9 @@
     <row r="61">
       <c r="A61" s="1">
         <v>60.0</v>
+      </c>
+      <c r="B61" s="1">
+        <v>9.0</v>
       </c>
       <c r="C61" s="1">
         <v>23.0</v>

</xml_diff>

<commit_message>
22/11/2020: fixed timestamp issue when import xlsx file to database
</commit_message>
<xml_diff>
--- a/ExcelTables/GetLad.xlsx
+++ b/ExcelTables/GetLad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="240">
   <si>
     <t>ID</t>
   </si>
@@ -47,6 +47,12 @@
     <t>Michael123</t>
   </si>
   <si>
+    <t>2020/11/13</t>
+  </si>
+  <si>
+    <t>2020/11/22</t>
+  </si>
+  <si>
     <t>Vincent</t>
   </si>
   <si>
@@ -56,6 +62,12 @@
     <t>Vincent123</t>
   </si>
   <si>
+    <t>2020/11/21</t>
+  </si>
+  <si>
+    <t>2020/11/23</t>
+  </si>
+  <si>
     <t>Harriat</t>
   </si>
   <si>
@@ -65,6 +77,9 @@
     <t>Harriat123</t>
   </si>
   <si>
+    <t>2020/11/12</t>
+  </si>
+  <si>
     <t>Molly</t>
   </si>
   <si>
@@ -74,6 +89,12 @@
     <t>Molly123</t>
   </si>
   <si>
+    <t>2020/11/19</t>
+  </si>
+  <si>
+    <t>2020/11/25</t>
+  </si>
+  <si>
     <t>Ken</t>
   </si>
   <si>
@@ -83,6 +104,12 @@
     <t>Ken123</t>
   </si>
   <si>
+    <t>2020/11/18</t>
+  </si>
+  <si>
+    <t>2020/11/26</t>
+  </si>
+  <si>
     <t>Kelvin</t>
   </si>
   <si>
@@ -92,6 +119,12 @@
     <t>Kelvin123</t>
   </si>
   <si>
+    <t>2020/11/17</t>
+  </si>
+  <si>
+    <t>2020/11/27</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
@@ -101,6 +134,12 @@
     <t>John123</t>
   </si>
   <si>
+    <t>2020/11/16</t>
+  </si>
+  <si>
+    <t>2020/11/28</t>
+  </si>
+  <si>
     <t>Donald</t>
   </si>
   <si>
@@ -110,6 +149,12 @@
     <t>Donald123</t>
   </si>
   <si>
+    <t>2020/11/15</t>
+  </si>
+  <si>
+    <t>2020/11/29</t>
+  </si>
+  <si>
     <t>Susan</t>
   </si>
   <si>
@@ -119,6 +164,12 @@
     <t>Susan123</t>
   </si>
   <si>
+    <t>2020/11/14</t>
+  </si>
+  <si>
+    <t>2020/11/30</t>
+  </si>
+  <si>
     <t>Mary</t>
   </si>
   <si>
@@ -137,6 +188,12 @@
     <t>Johnson123</t>
   </si>
   <si>
+    <t>2020/11/20</t>
+  </si>
+  <si>
+    <t>2020/11/24</t>
+  </si>
+  <si>
     <t>Jimmy</t>
   </si>
   <si>
@@ -146,6 +203,9 @@
     <t>Jimmy123</t>
   </si>
   <si>
+    <t>2020/11/11</t>
+  </si>
+  <si>
     <t>Conan</t>
   </si>
   <si>
@@ -155,6 +215,9 @@
     <t>Conan123</t>
   </si>
   <si>
+    <t>2020/11/10</t>
+  </si>
+  <si>
     <t>Christopher</t>
   </si>
   <si>
@@ -164,6 +227,9 @@
     <t>Christopher123</t>
   </si>
   <si>
+    <t>2020/11/9</t>
+  </si>
+  <si>
     <t>Debbie</t>
   </si>
   <si>
@@ -173,6 +239,9 @@
     <t>Debbie123</t>
   </si>
   <si>
+    <t>2020/11/8</t>
+  </si>
+  <si>
     <t>Fyen</t>
   </si>
   <si>
@@ -182,6 +251,9 @@
     <t>Fyen123</t>
   </si>
   <si>
+    <t>2020/11/7</t>
+  </si>
+  <si>
     <t>Paul</t>
   </si>
   <si>
@@ -191,6 +263,9 @@
     <t>Paul123</t>
   </si>
   <si>
+    <t>2020/11/6</t>
+  </si>
+  <si>
     <t>Adrain</t>
   </si>
   <si>
@@ -200,6 +275,9 @@
     <t>Adrain123</t>
   </si>
   <si>
+    <t>2020/11/5</t>
+  </si>
+  <si>
     <t>Adriann</t>
   </si>
   <si>
@@ -209,6 +287,9 @@
     <t>Adriann123</t>
   </si>
   <si>
+    <t>2020/11/4</t>
+  </si>
+  <si>
     <t>David</t>
   </si>
   <si>
@@ -218,6 +299,9 @@
     <t>David123</t>
   </si>
   <si>
+    <t>2020/11/3</t>
+  </si>
+  <si>
     <t>Eason</t>
   </si>
   <si>
@@ -227,6 +311,9 @@
     <t>Eason123</t>
   </si>
   <si>
+    <t>2020/11/2</t>
+  </si>
+  <si>
     <t>Matilda</t>
   </si>
   <si>
@@ -236,6 +323,9 @@
     <t>Matilda123</t>
   </si>
   <si>
+    <t>2020/11/1</t>
+  </si>
+  <si>
     <t>Benny</t>
   </si>
   <si>
@@ -245,6 +335,9 @@
     <t>Benny123</t>
   </si>
   <si>
+    <t>2020/10/31</t>
+  </si>
+  <si>
     <t>Phoebe</t>
   </si>
   <si>
@@ -254,6 +347,9 @@
     <t>Phoebe123</t>
   </si>
   <si>
+    <t>2020/10/30</t>
+  </si>
+  <si>
     <t>Anna</t>
   </si>
   <si>
@@ -263,6 +359,9 @@
     <t>Anna123</t>
   </si>
   <si>
+    <t>2020/10/29</t>
+  </si>
+  <si>
     <t>Daniel</t>
   </si>
   <si>
@@ -272,6 +371,9 @@
     <t>Daniel123</t>
   </si>
   <si>
+    <t>2020/10/28</t>
+  </si>
+  <si>
     <t>Ian</t>
   </si>
   <si>
@@ -281,6 +383,9 @@
     <t>Ian123</t>
   </si>
   <si>
+    <t>2020/10/27</t>
+  </si>
+  <si>
     <t>Sasha</t>
   </si>
   <si>
@@ -290,6 +395,9 @@
     <t>Sasha123</t>
   </si>
   <si>
+    <t>2020/10/26</t>
+  </si>
+  <si>
     <t>Audrey</t>
   </si>
   <si>
@@ -299,6 +407,9 @@
     <t>Audrey123</t>
   </si>
   <si>
+    <t>2020/10/25</t>
+  </si>
+  <si>
     <t>Franklin</t>
   </si>
   <si>
@@ -308,6 +419,9 @@
     <t>Franklin123</t>
   </si>
   <si>
+    <t>2020/10/24</t>
+  </si>
+  <si>
     <t>event_id</t>
   </si>
   <si>
@@ -555,6 +669,9 @@
   </si>
   <si>
     <t>活動: 有多两张门票 先到先得 (限女) 時間: 19:00 聯絡: 有意請致電: xxxx</t>
+  </si>
+  <si>
+    <t>2020/12/23</t>
   </si>
   <si>
     <t>红馆</t>
@@ -674,7 +791,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -957,11 +1074,11 @@
       <c r="E2" s="1">
         <v>0.0</v>
       </c>
-      <c r="F2" s="3">
-        <v>44148.0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>44157.0</v>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -969,22 +1086,22 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1">
         <v>0.0</v>
       </c>
-      <c r="F3" s="3">
-        <v>44156.0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>44158.0</v>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -992,22 +1109,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1">
         <v>0.0</v>
       </c>
-      <c r="F4" s="3">
-        <v>44147.0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>44158.0</v>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -1015,22 +1132,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
         <v>0.0</v>
       </c>
-      <c r="F5" s="3">
-        <v>44154.0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>44160.0</v>
+      <c r="F5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -1038,22 +1155,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1">
         <v>0.0</v>
       </c>
-      <c r="F6" s="3">
-        <v>44153.0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>44161.0</v>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7">
@@ -1061,22 +1178,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1">
         <v>0.0</v>
       </c>
-      <c r="F7" s="3">
-        <v>44152.0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>44162.0</v>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -1084,22 +1201,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1">
         <v>0.0</v>
       </c>
-      <c r="F8" s="3">
-        <v>44151.0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>44163.0</v>
+      <c r="F8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -1107,22 +1224,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1">
         <v>0.0</v>
       </c>
-      <c r="F9" s="3">
-        <v>44150.0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>44164.0</v>
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10">
@@ -1130,22 +1247,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1">
         <v>0.0</v>
       </c>
-      <c r="F10" s="3">
-        <v>44149.0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>44165.0</v>
+      <c r="F10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11">
@@ -1153,22 +1270,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1">
         <v>0.0</v>
       </c>
-      <c r="F11" s="3">
-        <v>44157.0</v>
-      </c>
-      <c r="G11" s="3">
-        <v>44157.0</v>
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12">
@@ -1176,22 +1293,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1">
         <v>0.0</v>
       </c>
-      <c r="F12" s="3">
-        <v>44155.0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>44159.0</v>
+      <c r="F12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -1199,22 +1316,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1">
         <v>0.0</v>
       </c>
-      <c r="F13" s="3">
-        <v>44146.0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>44159.0</v>
+      <c r="F13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -1222,22 +1339,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1">
         <v>0.0</v>
       </c>
-      <c r="F14" s="3">
-        <v>44145.0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>44160.0</v>
+      <c r="F14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -1245,22 +1362,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="E15" s="1">
         <v>0.0</v>
       </c>
-      <c r="F15" s="3">
-        <v>44144.0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>44161.0</v>
+      <c r="F15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -1268,22 +1385,22 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="E16" s="1">
         <v>0.0</v>
       </c>
-      <c r="F16" s="3">
-        <v>44143.0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>44162.0</v>
+      <c r="F16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -1291,22 +1408,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E17" s="1">
         <v>0.0</v>
       </c>
-      <c r="F17" s="3">
-        <v>44142.0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>44163.0</v>
+      <c r="F17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18">
@@ -1314,22 +1431,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E18" s="1">
         <v>0.0</v>
       </c>
-      <c r="F18" s="3">
-        <v>44141.0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>44164.0</v>
+      <c r="F18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19">
@@ -1337,22 +1454,22 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1">
         <v>0.0</v>
       </c>
-      <c r="F19" s="3">
-        <v>44140.0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>44165.0</v>
+      <c r="F19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20">
@@ -1360,22 +1477,22 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1">
         <v>0.0</v>
       </c>
-      <c r="F20" s="3">
-        <v>44139.0</v>
-      </c>
-      <c r="G20" s="4">
-        <v>44157.0</v>
+      <c r="F20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21">
@@ -1383,22 +1500,22 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="E21" s="1">
         <v>0.0</v>
       </c>
-      <c r="F21" s="3">
-        <v>44138.0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>44158.0</v>
+      <c r="F21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -1406,22 +1523,22 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="E22" s="1">
         <v>0.0</v>
       </c>
-      <c r="F22" s="3">
-        <v>44137.0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>44159.0</v>
+      <c r="F22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23">
@@ -1429,22 +1546,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="E23" s="1">
         <v>0.0</v>
       </c>
-      <c r="F23" s="3">
-        <v>44136.0</v>
-      </c>
-      <c r="G23" s="4">
-        <v>44160.0</v>
+      <c r="F23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1452,22 +1569,22 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="E24" s="1">
         <v>0.0</v>
       </c>
-      <c r="F24" s="3">
-        <v>44135.0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>44161.0</v>
+      <c r="F24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25">
@@ -1475,22 +1592,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="E25" s="1">
         <v>0.0</v>
       </c>
-      <c r="F25" s="3">
-        <v>44134.0</v>
-      </c>
-      <c r="G25" s="4">
-        <v>44162.0</v>
+      <c r="F25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26">
@@ -1498,22 +1615,22 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="E26" s="1">
         <v>0.0</v>
       </c>
-      <c r="F26" s="3">
-        <v>44133.0</v>
-      </c>
-      <c r="G26" s="4">
-        <v>44163.0</v>
+      <c r="F26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27">
@@ -1521,22 +1638,22 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="E27" s="1">
         <v>0.0</v>
       </c>
-      <c r="F27" s="3">
-        <v>44132.0</v>
-      </c>
-      <c r="G27" s="4">
-        <v>44164.0</v>
+      <c r="F27" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28">
@@ -1544,22 +1661,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="E28" s="1">
         <v>0.0</v>
       </c>
-      <c r="F28" s="3">
-        <v>44131.0</v>
-      </c>
-      <c r="G28" s="4">
-        <v>44165.0</v>
+      <c r="F28" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="29">
@@ -1567,22 +1684,22 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>90</v>
+        <v>125</v>
       </c>
       <c r="E29" s="1">
         <v>0.0</v>
       </c>
-      <c r="F29" s="3">
-        <v>44130.0</v>
-      </c>
-      <c r="G29" s="4">
-        <v>44157.0</v>
+      <c r="F29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -1590,22 +1707,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="E30" s="1">
         <v>0.0</v>
       </c>
-      <c r="F30" s="3">
-        <v>44129.0</v>
-      </c>
-      <c r="G30" s="4">
-        <v>44158.0</v>
+      <c r="F30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -1613,22 +1730,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="E31" s="1">
         <v>0.0</v>
       </c>
-      <c r="F31" s="3">
-        <v>44128.0</v>
-      </c>
-      <c r="G31" s="4">
-        <v>44159.0</v>
+      <c r="F31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32">
@@ -1669,10 +1786,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
@@ -2795,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2">
@@ -3485,31 +3602,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
@@ -3520,16 +3637,16 @@
         <v>21.0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44158.0</v>
+        <v>146</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="G2" s="2">
         <v>3.0</v>
@@ -3546,16 +3663,16 @@
         <v>13.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="3">
-        <v>44164.0</v>
+        <v>149</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="G3" s="1">
         <v>5.0</v>
@@ -3572,16 +3689,16 @@
         <v>23.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="3">
-        <v>44160.0</v>
+        <v>152</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="G4" s="1">
         <v>9.0</v>
@@ -3598,16 +3715,16 @@
         <v>23.0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="3">
-        <v>44162.0</v>
+        <v>155</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="G5" s="1">
         <v>6.0</v>
@@ -3624,16 +3741,16 @@
         <v>17.0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="3">
-        <v>44157.0</v>
+        <v>158</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>121</v>
+        <v>159</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="G6" s="2">
         <v>2.0</v>
@@ -3650,16 +3767,16 @@
         <v>24.0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="3">
-        <v>44159.0</v>
+        <v>161</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="G7" s="2">
         <v>4.0</v>
@@ -3676,16 +3793,16 @@
         <v>20.0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="3">
-        <v>44162.0</v>
+        <v>163</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="G8" s="2">
         <v>11.0</v>
@@ -3702,16 +3819,16 @@
         <v>19.0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="3">
-        <v>44160.0</v>
+        <v>166</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="G9" s="1">
         <v>3.0</v>
@@ -3728,16 +3845,16 @@
         <v>10.0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="3">
-        <v>44163.0</v>
+        <v>169</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="G10" s="1">
         <v>2.0</v>
@@ -3754,16 +3871,16 @@
         <v>4.0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="3">
-        <v>44161.0</v>
+        <v>172</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="G11" s="1">
         <v>6.0</v>
@@ -3780,16 +3897,16 @@
         <v>20.0</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D12" s="3">
-        <v>44159.0</v>
+        <v>175</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>138</v>
+        <v>176</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="G12" s="1">
         <v>9.0</v>
@@ -3806,16 +3923,16 @@
         <v>17.0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D13" s="3">
-        <v>44159.0</v>
+        <v>178</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>142</v>
+        <v>180</v>
       </c>
       <c r="G13" s="2">
         <v>2.0</v>
@@ -3832,16 +3949,16 @@
         <v>12.0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="3">
-        <v>44162.0</v>
+        <v>181</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="G14" s="1">
         <v>3.0</v>
@@ -3858,16 +3975,16 @@
         <v>14.0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" s="3">
-        <v>44163.0</v>
+        <v>184</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>147</v>
+        <v>185</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="G15" s="1">
         <v>6.0</v>
@@ -3884,16 +4001,16 @@
         <v>22.0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="3">
-        <v>44161.0</v>
+        <v>187</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="G16" s="2">
         <v>4.0</v>
@@ -3910,16 +4027,16 @@
         <v>16.0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="3">
-        <v>44158.0</v>
+        <v>190</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="G17" s="1">
         <v>9.0</v>
@@ -3936,16 +4053,16 @@
         <v>15.0</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="3">
-        <v>44164.0</v>
+        <v>193</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>157</v>
+        <v>195</v>
       </c>
       <c r="G18" s="2">
         <v>3.0</v>
@@ -3962,16 +4079,16 @@
         <v>1.0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D19" s="3">
-        <v>44157.0</v>
+        <v>196</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>159</v>
+        <v>197</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="G19" s="2">
         <v>3.0</v>
@@ -3988,16 +4105,16 @@
         <v>3.0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D20" s="3">
-        <v>44158.0</v>
+        <v>199</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="G20" s="2">
         <v>4.0</v>
@@ -4014,16 +4131,16 @@
         <v>18.0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="D21" s="3">
-        <v>44158.0</v>
+        <v>202</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>165</v>
+        <v>203</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="G21" s="2">
         <v>2.0</v>
@@ -4040,16 +4157,16 @@
         <v>25.0</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D22" s="3">
-        <v>44157.0</v>
+        <v>205</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="G22" s="2">
         <v>4.0</v>
@@ -4066,16 +4183,16 @@
         <v>24.0</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" s="3">
-        <v>44157.0</v>
+        <v>208</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="G23" s="1">
         <v>10.0</v>
@@ -4092,16 +4209,16 @@
         <v>18.0</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D24" s="3">
-        <v>44159.0</v>
+        <v>211</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="G24" s="1">
         <v>7.0</v>
@@ -4118,16 +4235,16 @@
         <v>11.0</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D25" s="3">
-        <v>44164.0</v>
+        <v>214</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>177</v>
+        <v>215</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="G25" s="1">
         <v>3.0</v>
@@ -4144,16 +4261,16 @@
         <v>19.0</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D26" s="4">
-        <v>44188.0</v>
+        <v>217</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="G26" s="2">
         <v>3.0</v>
@@ -4170,16 +4287,16 @@
         <v>16.0</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D27" s="4">
-        <v>44165.0</v>
+        <v>221</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="G27" s="1">
         <v>4.0</v>
@@ -4196,16 +4313,16 @@
         <v>15.0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D28" s="3">
-        <v>44160.0</v>
+        <v>224</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>186</v>
+        <v>225</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>187</v>
+        <v>226</v>
       </c>
       <c r="G28" s="2">
         <v>8.0</v>
@@ -4222,16 +4339,16 @@
         <v>9.0</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D29" s="3">
-        <v>44165.0</v>
+        <v>227</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>189</v>
+        <v>228</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>190</v>
+        <v>229</v>
       </c>
       <c r="G29" s="2">
         <v>2.0</v>
@@ -4248,16 +4365,16 @@
         <v>27.0</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D30" s="3">
-        <v>44165.0</v>
+        <v>230</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="G30" s="1">
         <v>8.0</v>
@@ -4274,16 +4391,16 @@
         <v>22.0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D31" s="3">
-        <v>44165.0</v>
+        <v>233</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>196</v>
+        <v>235</v>
       </c>
       <c r="G31" s="1">
         <v>2.0</v>
@@ -4312,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2">
@@ -4320,7 +4437,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
@@ -4328,7 +4445,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4">
@@ -4336,7 +4453,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed excel tables and insertTableFromExcel bugs
</commit_message>
<xml_diff>
--- a/ExcelTables/GetLad.xlsx
+++ b/ExcelTables/GetLad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="240">
   <si>
     <t>ID</t>
   </si>
@@ -449,7 +449,7 @@
     <t>prerequisite</t>
   </si>
   <si>
-    <t>event_type</t>
+    <t>event_type_id</t>
   </si>
   <si>
     <t>updated_at</t>
@@ -781,20 +781,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1045,7 +1048,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1059,7 +1062,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1074,10 +1077,10 @@
       <c r="E2" s="1">
         <v>0.0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1085,10 +1088,10 @@
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1097,21 +1100,21 @@
       <c r="E3" s="1">
         <v>0.0</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1120,10 +1123,10 @@
       <c r="E4" s="1">
         <v>0.0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1134,7 +1137,7 @@
       <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1143,10 +1146,10 @@
       <c r="E5" s="1">
         <v>0.0</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1157,7 +1160,7 @@
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1166,10 +1169,10 @@
       <c r="E6" s="1">
         <v>0.0</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1180,7 +1183,7 @@
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1189,10 +1192,10 @@
       <c r="E7" s="1">
         <v>0.0</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1203,7 +1206,7 @@
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1212,10 +1215,10 @@
       <c r="E8" s="1">
         <v>0.0</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1226,7 +1229,7 @@
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1235,10 +1238,10 @@
       <c r="E9" s="1">
         <v>0.0</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1249,7 +1252,7 @@
       <c r="B10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1258,15 +1261,15 @@
       <c r="E10" s="1">
         <v>0.0</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1281,15 +1284,15 @@
       <c r="E11" s="1">
         <v>0.0</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>11.0</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1304,10 +1307,10 @@
       <c r="E12" s="1">
         <v>0.0</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1318,7 +1321,7 @@
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1327,10 +1330,10 @@
       <c r="E13" s="1">
         <v>0.0</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1341,7 +1344,7 @@
       <c r="B14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1350,10 +1353,10 @@
       <c r="E14" s="1">
         <v>0.0</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1364,7 +1367,7 @@
       <c r="B15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1373,10 +1376,10 @@
       <c r="E15" s="1">
         <v>0.0</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1387,7 +1390,7 @@
       <c r="B16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1396,10 +1399,10 @@
       <c r="E16" s="1">
         <v>0.0</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1410,7 +1413,7 @@
       <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1419,10 +1422,10 @@
       <c r="E17" s="1">
         <v>0.0</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1433,7 +1436,7 @@
       <c r="B18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1442,10 +1445,10 @@
       <c r="E18" s="1">
         <v>0.0</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1456,7 +1459,7 @@
       <c r="B19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1465,10 +1468,10 @@
       <c r="E19" s="1">
         <v>0.0</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1476,10 +1479,10 @@
       <c r="A20" s="1">
         <v>19.0</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1488,10 +1491,10 @@
       <c r="E20" s="1">
         <v>0.0</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1502,7 +1505,7 @@
       <c r="B21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1511,10 +1514,10 @@
       <c r="E21" s="1">
         <v>0.0</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1525,7 +1528,7 @@
       <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1534,10 +1537,10 @@
       <c r="E22" s="1">
         <v>0.0</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1548,7 +1551,7 @@
       <c r="B23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1557,10 +1560,10 @@
       <c r="E23" s="1">
         <v>0.0</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1571,7 +1574,7 @@
       <c r="B24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1580,10 +1583,10 @@
       <c r="E24" s="1">
         <v>0.0</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1594,7 +1597,7 @@
       <c r="B25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1603,10 +1606,10 @@
       <c r="E25" s="1">
         <v>0.0</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1617,7 +1620,7 @@
       <c r="B26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -1626,10 +1629,10 @@
       <c r="E26" s="1">
         <v>0.0</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1640,7 +1643,7 @@
       <c r="B27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1649,10 +1652,10 @@
       <c r="E27" s="1">
         <v>0.0</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1663,7 +1666,7 @@
       <c r="B28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>120</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1672,10 +1675,10 @@
       <c r="E28" s="1">
         <v>0.0</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1686,7 +1689,7 @@
       <c r="B29" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>124</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1695,10 +1698,10 @@
       <c r="E29" s="1">
         <v>0.0</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1709,7 +1712,7 @@
       <c r="B30" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1718,10 +1721,10 @@
       <c r="E30" s="1">
         <v>0.0</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1732,7 +1735,7 @@
       <c r="B31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -1741,30 +1744,30 @@
       <c r="E31" s="1">
         <v>0.0</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="32">
-      <c r="G32" s="4"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33">
-      <c r="G33" s="4"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34">
-      <c r="G34" s="4"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35">
-      <c r="G35" s="4"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36">
-      <c r="G36" s="4"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37">
-      <c r="G37" s="4"/>
+      <c r="G37" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2049,7 +2052,7 @@
       <c r="A25" s="1">
         <v>24.0</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>27.0</v>
       </c>
       <c r="C25" s="1">
@@ -2082,7 +2085,7 @@
       <c r="A28" s="1">
         <v>27.0</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>28.0</v>
       </c>
       <c r="C28" s="1">
@@ -2236,7 +2239,7 @@
       <c r="A42" s="1">
         <v>41.0</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>30.0</v>
       </c>
       <c r="C42" s="1">
@@ -2269,7 +2272,7 @@
       <c r="A45" s="1">
         <v>44.0</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>29.0</v>
       </c>
       <c r="C45" s="1">
@@ -2456,7 +2459,7 @@
       <c r="A62" s="1">
         <v>61.0</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>25.0</v>
       </c>
       <c r="C62" s="1">
@@ -2874,7 +2877,7 @@
       <c r="A100" s="1">
         <v>99.0</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>26.0</v>
       </c>
       <c r="C100" s="1">
@@ -3613,19 +3616,19 @@
       <c r="E1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3636,23 +3639,29 @@
       <c r="B2" s="1">
         <v>21.0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>3.0</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -3662,23 +3671,29 @@
       <c r="B3" s="1">
         <v>13.0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <v>5.0</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4">
@@ -3688,23 +3703,29 @@
       <c r="B4" s="1">
         <v>23.0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="4">
         <v>9.0</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -3714,23 +3735,29 @@
       <c r="B5" s="1">
         <v>23.0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="4">
         <v>6.0</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -3740,23 +3767,29 @@
       <c r="B6" s="1">
         <v>17.0</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>2.0</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
@@ -3766,23 +3799,29 @@
       <c r="B7" s="1">
         <v>24.0</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>4.0</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -3792,23 +3831,29 @@
       <c r="B8" s="1">
         <v>20.0</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>11.0</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -3818,23 +3863,29 @@
       <c r="B9" s="1">
         <v>19.0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="4">
         <v>3.0</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -3844,23 +3895,29 @@
       <c r="B10" s="1">
         <v>10.0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="4">
         <v>2.0</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -3870,23 +3927,29 @@
       <c r="B11" s="1">
         <v>4.0</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="4">
         <v>6.0</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12">
@@ -3896,23 +3959,29 @@
       <c r="B12" s="1">
         <v>20.0</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>9.0</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -3922,23 +3991,29 @@
       <c r="B13" s="1">
         <v>17.0</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="4">
         <v>2.0</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -3948,23 +4023,29 @@
       <c r="B14" s="1">
         <v>12.0</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="4">
         <v>3.0</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -3974,23 +4055,29 @@
       <c r="B15" s="1">
         <v>14.0</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="4">
         <v>6.0</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16">
@@ -4000,23 +4087,29 @@
       <c r="B16" s="1">
         <v>22.0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="4">
         <v>4.0</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="17">
@@ -4026,23 +4119,29 @@
       <c r="B17" s="1">
         <v>16.0</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="4">
         <v>9.0</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -4052,23 +4151,29 @@
       <c r="B18" s="1">
         <v>15.0</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="4">
         <v>3.0</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19">
@@ -4078,23 +4183,29 @@
       <c r="B19" s="1">
         <v>1.0</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="4">
         <v>3.0</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -4104,23 +4215,29 @@
       <c r="B20" s="1">
         <v>3.0</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="4">
         <v>4.0</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21">
@@ -4130,23 +4247,29 @@
       <c r="B21" s="1">
         <v>18.0</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="4">
         <v>2.0</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -4156,23 +4279,29 @@
       <c r="B22" s="1">
         <v>25.0</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="4">
         <v>4.0</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -4182,23 +4311,29 @@
       <c r="B23" s="1">
         <v>24.0</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="4">
         <v>10.0</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24">
@@ -4208,23 +4343,29 @@
       <c r="B24" s="1">
         <v>18.0</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="4">
         <v>7.0</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25">
@@ -4234,23 +4375,29 @@
       <c r="B25" s="1">
         <v>11.0</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="4">
         <v>3.0</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26">
@@ -4260,23 +4407,29 @@
       <c r="B26" s="1">
         <v>19.0</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>218</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="4">
         <v>3.0</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="27">
@@ -4286,23 +4439,29 @@
       <c r="B27" s="1">
         <v>16.0</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="4">
         <v>4.0</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="4">
         <v>1.0</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -4312,23 +4471,29 @@
       <c r="B28" s="1">
         <v>15.0</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="4">
         <v>8.0</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="29">
@@ -4338,23 +4503,29 @@
       <c r="B29" s="1">
         <v>9.0</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="4">
         <v>2.0</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="30">
@@ -4367,20 +4538,26 @@
       <c r="C30" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="4">
         <v>8.0</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="4">
         <v>2.0</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="31">
@@ -4390,23 +4567,29 @@
       <c r="B31" s="1">
         <v>22.0</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="4">
         <v>2.0</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="4">
         <v>3.0</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>